<commit_message>
SQL queries were modified for Lesson 4
</commit_message>
<xml_diff>
--- a/AndyTEST/Libs/UserStoriesChecklist.xlsx
+++ b/AndyTEST/Libs/UserStoriesChecklist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Story 1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
   <si>
     <t>Story 1</t>
   </si>
@@ -81,21 +81,12 @@
     <t>SELECT additionalSpaceService FROM</t>
   </si>
   <si>
-    <t>SELECT flightNumber FROM Flights WHERE departureAirport = 'New York';</t>
-  </si>
-  <si>
     <t>1005;1006;1007;1008;1009;1010;</t>
   </si>
   <si>
-    <t>SELECT flightNumber FROM Flights WHERE departureAirport = 'New York' AND stopsNumber = 0;</t>
-  </si>
-  <si>
     <t>1008;</t>
   </si>
   <si>
-    <t>SELECT flightNumber FROM Flights WHERE averageTicketPrice &lt; 500 AND departureAirport = 'New York';</t>
-  </si>
-  <si>
     <t>1006;1007;1008;1009;1010;</t>
   </si>
   <si>
@@ -117,9 +108,6 @@
     <t>Check the flight from New York and where the Duty Free shops are in the destination airport.</t>
   </si>
   <si>
-    <t>SELECT flightNumber FROM Flights INNER JOIN Airports ON Flights.airportNumber = Airports.airportNumber WHERE departureAirport = 'New York' AND dutyFree = 'yes';</t>
-  </si>
-  <si>
     <t>1006;1007;1008;1009;</t>
   </si>
   <si>
@@ -138,118 +126,64 @@
     <t>SELECT priorityBoarding FROM Airports WHERE airport = 'London';</t>
   </si>
   <si>
-    <t>SELECT Flights.flightNumber FROM Flights INNER JOIN Airlines ON Flights.flightNumber = Airlines.flightNumber WHERE departureAirport = 'New York' AND isMealincluded = 'yes';</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SELECT airline FROM Airlines INNER JOIN Flights ON Airlines.flightNumber = Flights.flightNumber WHERE arrivalAirport = 'Milan' </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>AND / OR</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> arrivalAirport = 'Helsinki';</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>SELECT airline FROM Airlines INNER JOIN Flights ON Airlines.flightNumber = Flights.flightNumber WHERE</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ( </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">arrivalAirport = 'Milan' </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>AND / OR</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> arrivalAirport = 'Helsinki' </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>AND webRegistration = 'yes';</t>
-    </r>
-  </si>
-  <si>
     <t>Lufthansa;Windrose Aero;Cathay Pacific;Virgin;Emirates;Windrose Aero;AirAsia;Emirates;Air France;</t>
   </si>
   <si>
     <t>Lufthansa;Cathay Pacific;Virgin;Emirates;Emirates;</t>
+  </si>
+  <si>
+    <t>-- SHow airlines which have ticket price less 100 Euro
+SELECT airline FROM Airlines
+INNER JOIN Flights
+ON Airlines.flightNumber = Flights.flightNumber
+WHERE averageTicketPrice &lt; 100
+GROUP BY airline
+-- Show airline which have average ticket price less 100 Euro
+SELECT airline FROM Airlines
+INNER JOIN Flights
+ON Airlines.flightNumber = Flights.flightNumber
+GROUP BY airline
+HAVING AVG(averageTicketPrice) &lt; 100</t>
+  </si>
+  <si>
+    <t>Air France
+AirAsia
+Austrian Airlines
+Cathay Pacific
+Emirates
+Lufthansa
+Ryanair
+Turkish Airlines
+Windrose Aero
+WizzAir                                                                                                      *                                     *                                 *                                  *                                        *                                          *                                        *                                                 *                                             *                                Turkish Airlines</t>
+  </si>
+  <si>
+    <t>SELECT airline FROM Airlines INNER JOIN Flights ON Airlines.flightNumber = Flights.flightNumber WHERE arrivalAirport IN ('Milan' , 'Helsinki' ) AND webRegistration = 'yes' GROUP BY airline</t>
+  </si>
+  <si>
+    <t>SELECT airline FROM Airlines INNER JOIN Flights ON Airlines.flightNumber = Flights.flightNumber WHERE arrivalAirport IN('Milan', 'Helsinki') GROUP BY airline</t>
+  </si>
+  <si>
+    <t>SELECT flightNumber FROM Flights INNER JOIN Airports ON Flights.airportNumber = Airports.airportNumber WHERE departureAirport = 'New York' AND dutyFree = 'yes'</t>
+  </si>
+  <si>
+    <t>SELECT Flights.flightNumber FROM Flights INNER JOIN Airlines ON Flights.flightNumber = Airlines.flightNumber WHERE departureAirport = 'New York' AND isMealincluded = 'yes'</t>
+  </si>
+  <si>
+    <t>SELECT flightNumber FROM Flights WHERE averageTicketPrice &lt; 500 AND departureAirport = 'New York'</t>
+  </si>
+  <si>
+    <t>SELECT flightNumber FROM Flights WHERE departureAirport = 'New York' AND stopsNumber = 0</t>
+  </si>
+  <si>
+    <t>SELECT flightNumber FROM Flights WHERE departureAirport = 'New York'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,15 +204,6 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -338,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -385,6 +310,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -693,7 +621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -757,10 +685,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>15</v>
@@ -1049,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1097,13 +1025,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C3" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>21</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>22</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -1113,13 +1041,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
@@ -1129,13 +1057,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
@@ -1145,13 +1073,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
@@ -1161,13 +1089,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
@@ -1407,7 +1335,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1454,13 +1382,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>41</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -1470,26 +1398,30 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="315" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
+        <v>33</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>39</v>
+      </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
     </row>

</xml_diff>

<commit_message>
Worked with Excels cells and ArrayList of arrays.
</commit_message>
<xml_diff>
--- a/AndyTEST/Libs/UserStoriesChecklist.xlsx
+++ b/AndyTEST/Libs/UserStoriesChecklist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Story 1" sheetId="1" r:id="rId1"/>
@@ -132,13 +132,28 @@
     <t>Lufthansa;Cathay Pacific;Virgin;Emirates;Emirates;</t>
   </si>
   <si>
-    <t>-- SHow airlines which have ticket price less 100 Euro
-SELECT airline FROM Airlines
-INNER JOIN Flights
-ON Airlines.flightNumber = Flights.flightNumber
-WHERE averageTicketPrice &lt; 100
-GROUP BY airline
--- Show airline which have average ticket price less 100 Euro
+    <t>SELECT airline FROM Airlines INNER JOIN Flights ON Airlines.flightNumber = Flights.flightNumber WHERE arrivalAirport IN ('Milan' , 'Helsinki' ) AND webRegistration = 'yes' GROUP BY airline</t>
+  </si>
+  <si>
+    <t>SELECT airline FROM Airlines INNER JOIN Flights ON Airlines.flightNumber = Flights.flightNumber WHERE arrivalAirport IN('Milan', 'Helsinki') GROUP BY airline</t>
+  </si>
+  <si>
+    <t>SELECT flightNumber FROM Flights INNER JOIN Airports ON Flights.airportNumber = Airports.airportNumber WHERE departureAirport = 'New York' AND dutyFree = 'yes'</t>
+  </si>
+  <si>
+    <t>SELECT Flights.flightNumber FROM Flights INNER JOIN Airlines ON Flights.flightNumber = Airlines.flightNumber WHERE departureAirport = 'New York' AND isMealincluded = 'yes'</t>
+  </si>
+  <si>
+    <t>SELECT flightNumber FROM Flights WHERE averageTicketPrice &lt; 500 AND departureAirport = 'New York'</t>
+  </si>
+  <si>
+    <t>SELECT flightNumber FROM Flights WHERE departureAirport = 'New York' AND stopsNumber = 0</t>
+  </si>
+  <si>
+    <t>SELECT flightNumber FROM Flights WHERE departureAirport = 'New York'</t>
+  </si>
+  <si>
+    <t>price less 100 Euro
 SELECT airline FROM Airlines
 INNER JOIN Flights
 ON Airlines.flightNumber = Flights.flightNumber
@@ -146,44 +161,14 @@
 HAVING AVG(averageTicketPrice) &lt; 100</t>
   </si>
   <si>
-    <t>Air France
-AirAsia
-Austrian Airlines
-Cathay Pacific
-Emirates
-Lufthansa
-Ryanair
-Turkish Airlines
-Windrose Aero
-WizzAir                                                                                                      *                                     *                                 *                                  *                                        *                                          *                                        *                                                 *                                             *                                Turkish Airlines</t>
-  </si>
-  <si>
-    <t>SELECT airline FROM Airlines INNER JOIN Flights ON Airlines.flightNumber = Flights.flightNumber WHERE arrivalAirport IN ('Milan' , 'Helsinki' ) AND webRegistration = 'yes' GROUP BY airline</t>
-  </si>
-  <si>
-    <t>SELECT airline FROM Airlines INNER JOIN Flights ON Airlines.flightNumber = Flights.flightNumber WHERE arrivalAirport IN('Milan', 'Helsinki') GROUP BY airline</t>
-  </si>
-  <si>
-    <t>SELECT flightNumber FROM Flights INNER JOIN Airports ON Flights.airportNumber = Airports.airportNumber WHERE departureAirport = 'New York' AND dutyFree = 'yes'</t>
-  </si>
-  <si>
-    <t>SELECT Flights.flightNumber FROM Flights INNER JOIN Airlines ON Flights.flightNumber = Airlines.flightNumber WHERE departureAirport = 'New York' AND isMealincluded = 'yes'</t>
-  </si>
-  <si>
-    <t>SELECT flightNumber FROM Flights WHERE averageTicketPrice &lt; 500 AND departureAirport = 'New York'</t>
-  </si>
-  <si>
-    <t>SELECT flightNumber FROM Flights WHERE departureAirport = 'New York' AND stopsNumber = 0</t>
-  </si>
-  <si>
-    <t>SELECT flightNumber FROM Flights WHERE departureAirport = 'New York'</t>
+    <t>Turkish Airlines</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,6 +194,13 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -231,7 +223,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -263,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -303,9 +295,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -314,6 +303,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -621,7 +616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -684,7 +679,7 @@
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>34</v>
       </c>
       <c r="C4" s="12" t="s">
@@ -1028,7 +1023,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>21</v>
@@ -1044,7 +1039,7 @@
         <v>27</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>22</v>
@@ -1056,11 +1051,11 @@
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>44</v>
+      <c r="C5" s="16" t="s">
+        <v>42</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>23</v>
@@ -1075,8 +1070,8 @@
       <c r="B6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>43</v>
+      <c r="C6" s="16" t="s">
+        <v>41</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>24</v>
@@ -1092,7 +1087,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>30</v>
@@ -1334,8 +1329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1384,8 +1379,8 @@
       <c r="B3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>41</v>
+      <c r="C3" s="16" t="s">
+        <v>39</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>36</v>
@@ -1401,7 +1396,7 @@
         <v>32</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>37</v>
@@ -1409,18 +1404,18 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:6" ht="315" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>38</v>
+      <c r="C5" s="17" t="s">
+        <v>45</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
@@ -1516,7 +1511,7 @@
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
-      <c r="C17" s="2"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>

</xml_diff>